<commit_message>
added 3 new graphs about loops
</commit_message>
<xml_diff>
--- a/loops/Study.xlsx
+++ b/loops/Study.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="collections" sheetId="5" r:id="rId1"/>
@@ -2042,7 +2042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -15155,7 +15157,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -15169,7 +15170,7 @@
   <dimension ref="A1:AB91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23032,7 +23033,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AD91">
-    <sortState ref="A2:AC91">
+    <sortState ref="A2:AB91">
       <sortCondition ref="A1:A91"/>
     </sortState>
   </autoFilter>
@@ -23052,8 +23053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB238"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -43558,7 +43559,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AB238">
-    <sortState ref="A2:AC238">
+    <sortState ref="A2:AB238">
       <sortCondition ref="A1:A238"/>
     </sortState>
   </autoFilter>

</xml_diff>